<commit_message>
Fix quarter day overlap by merging overlapping project date ranges
Co-authored-by: colina83 <13612603+colina83@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Quarterly_Review_Breakdown.xlsx
+++ b/Quarterly_Review_Breakdown.xlsx
@@ -2420,7 +2420,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -2438,7 +2438,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
@@ -2474,7 +2474,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
@@ -2514,7 +2514,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" t="n">
         <v>437225</v>
@@ -2536,7 +2536,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
@@ -2554,7 +2554,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -2592,7 +2592,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
@@ -2612,7 +2612,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
@@ -2630,7 +2630,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
@@ -2684,7 +2684,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
@@ -2704,7 +2704,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
@@ -2722,7 +2722,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>148</v>
+        <v>67</v>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
@@ -2740,7 +2740,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
@@ -2776,7 +2776,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
@@ -2794,7 +2794,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>81</v>
+        <v>15</v>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
@@ -2830,7 +2830,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
@@ -2848,7 +2848,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
@@ -2866,7 +2866,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
@@ -2884,7 +2884,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
@@ -2938,7 +2938,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
@@ -3090,13 +3090,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -3108,7 +3108,7 @@
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G4" t="n">
         <v>437225</v>
@@ -3141,13 +3141,13 @@
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
@@ -3176,13 +3176,13 @@
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
@@ -3238,7 +3238,7 @@
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="n">
@@ -3259,19 +3259,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>148</v>
+        <v>67</v>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
@@ -3296,13 +3296,13 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="n">
-        <v>81</v>
+        <v>15</v>
       </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
@@ -3358,19 +3358,19 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="n">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
@@ -3383,7 +3383,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -3401,7 +3401,7 @@
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="n">

</xml_diff>